<commit_message>
KIBON-2271: TFO Rechner Luzern Verguenstigung pro Stunden rechnen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/test/java/ch/dvbern/ebegu/rechner/BG_Rechner_Luzern_0.2_Stand_Mai22.xlsx
+++ b/ebegu-server/src/test/java/ch/dvbern/ebegu/rechner/BG_Rechner_Luzern_0.2_Stand_Mai22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ebegu\ebegu-server\src\test\java\ch\dvbern\ebegu\rechner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ebegu-server\src\test\java\ch\dvbern\ebegu\rechner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FEE6B2-F3B3-4B3C-81A7-8FD8E176997D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04ABF27E-B9EA-4DFF-9AF6-E884C44E7146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kita" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="87">
   <si>
     <t>Minimaltarif</t>
   </si>
@@ -264,15 +264,9 @@
     <t>Gutschein Pro Stunde vor Zuschläge, vor Selbstbehalt</t>
   </si>
   <si>
-    <t>Gutschein Pro Monat vor Zuschläge und Selbstbehalt</t>
-  </si>
-  <si>
     <t>Gutschein pro Stunde</t>
   </si>
   <si>
-    <t>Zuschlag pro Monat</t>
-  </si>
-  <si>
     <t>Vollkosten</t>
   </si>
   <si>
@@ -289,6 +283,21 @@
   </si>
   <si>
     <t>Kind 3</t>
+  </si>
+  <si>
+    <t>Zusätzlicher Selbstbehalt pro Tag</t>
+  </si>
+  <si>
+    <t>Differenz Vollkosten und Gutschein (pro Stunde)</t>
+  </si>
+  <si>
+    <t>Minimaler Selbstbehalt (pro Stunde)</t>
+  </si>
+  <si>
+    <t>Gutschein pro Stunde vor Zuschläge</t>
+  </si>
+  <si>
+    <t>Zuschlag pro Stunde</t>
   </si>
 </sst>
 </file>
@@ -299,7 +308,7 @@
     <numFmt numFmtId="164" formatCode="0.000000000000000"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="173" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -492,7 +501,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -713,16 +722,17 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="4" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="4" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="3"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1009,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4189,10 +4199,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCBD1BC8-8811-476C-8145-4E858DCA8165}">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K4" sqref="K1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4236,22 +4246,22 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C4" s="111" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D4" s="112"/>
       <c r="E4" s="111" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F4" s="113"/>
       <c r="G4" s="111" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H4" s="112"/>
       <c r="I4" s="111" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J4" s="111" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -4305,19 +4315,19 @@
         <v>50</v>
       </c>
       <c r="D7" s="122"/>
-      <c r="E7" s="121">
-        <v>30</v>
+      <c r="E7" s="139">
+        <v>30.75</v>
       </c>
       <c r="F7" s="123"/>
       <c r="G7" s="121">
         <v>150</v>
       </c>
       <c r="H7" s="122"/>
-      <c r="I7" s="141">
+      <c r="I7" s="138">
         <v>63</v>
       </c>
       <c r="J7" s="121">
-        <v>74.010000000000005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -4331,18 +4341,18 @@
         <v>45.1</v>
       </c>
       <c r="D8" s="122"/>
-      <c r="E8" s="139">
-        <v>22.55</v>
+      <c r="E8" s="137">
+        <v>67.650000000000006</v>
       </c>
       <c r="F8" s="123"/>
-      <c r="G8" s="139">
+      <c r="G8" s="137">
         <v>180.4</v>
       </c>
       <c r="H8" s="122"/>
-      <c r="I8" s="139">
+      <c r="I8" s="137">
         <v>112.75</v>
       </c>
-      <c r="J8" s="139">
+      <c r="J8" s="137">
         <v>90.2</v>
       </c>
     </row>
@@ -4466,28 +4476,28 @@
       <c r="A14" s="118" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="138">
+      <c r="C14" s="136">
         <f>(100/(($E$2/12)*$E$3))*C7</f>
         <v>22.172949002217297</v>
       </c>
       <c r="D14" s="112"/>
       <c r="E14" s="2">
         <f>(100/(($E$2/12)*$E$3))*E7</f>
-        <v>13.303769401330378</v>
+        <v>13.636363636363637</v>
       </c>
       <c r="F14" s="113"/>
-      <c r="G14" s="138">
+      <c r="G14" s="136">
         <f>(100/(($E$2/12)*$E$3))*G7</f>
         <v>66.518847006651882</v>
       </c>
       <c r="H14" s="112"/>
-      <c r="I14" s="138">
+      <c r="I14" s="136">
         <f>(100/(($E$2/12)*$E$3))*I7</f>
         <v>27.937915742793791</v>
       </c>
-      <c r="J14" s="138">
+      <c r="J14" s="136">
         <f t="shared" ref="J14" si="0">(100/(($E$2/12)*$E$3))*J7</f>
-        <v>32.820399113082047</v>
+        <v>0</v>
       </c>
       <c r="K14" t="s">
         <v>71</v>
@@ -4504,7 +4514,7 @@
       <c r="D15" s="112"/>
       <c r="E15" s="2">
         <f>(100/(($E$2/12)*$E$3))*E8</f>
-        <v>10</v>
+        <v>30.000000000000004</v>
       </c>
       <c r="F15" s="113"/>
       <c r="G15" s="2">
@@ -4917,21 +4927,21 @@
       </c>
       <c r="D34" s="133"/>
       <c r="E34" s="133">
-        <f>MIN((IF((E18*(1-E26))&gt;E30,(E18*(1-E26)),IF(E9&lt;=125000,E30,0))),E18-E17)</f>
+        <f t="shared" ref="D34:J34" si="7">MIN((IF((E18*(1-E26))&gt;E30,(E18*(1-E26)),IF(E9&lt;=125000,E30,0))),E18-E17)</f>
         <v>9.1168831168831179</v>
       </c>
-      <c r="F34" s="134"/>
+      <c r="F34" s="133"/>
       <c r="G34" s="133">
-        <f>MIN((IF((G18*(1-G26))&gt;G30,(G18*(1-G26)),IF(G9&lt;=125000,G30,0))),G18-G17)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H34" s="133"/>
       <c r="I34" s="133">
-        <f>MIN((IF((I18*(1-I26))&gt;I30,(I18*(1-I26)),IF(I9&lt;=125000,I30,0))),I18-I17)</f>
+        <f t="shared" si="7"/>
         <v>15.600000000000001</v>
       </c>
       <c r="J34" s="133">
-        <f>MIN((IF((J18*(1-J26))&gt;J30,(J18*(1-J26)),IF(J9&lt;=125000,J30,0))),J18-J17)</f>
+        <f t="shared" si="7"/>
         <v>7.5974025974025983</v>
       </c>
       <c r="K34" t="s">
@@ -4952,21 +4962,21 @@
       </c>
       <c r="D35" s="133"/>
       <c r="E35" s="133">
-        <f>IF(E11,E27,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="134"/>
+        <f t="shared" ref="D35:J35" si="8">IF(E11,E27,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="133"/>
       <c r="G35" s="133">
-        <f>IF(G11,G27,0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H35" s="133"/>
       <c r="I35" s="133">
-        <f>IF(I11,I27,0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J35" s="133">
-        <f>IF(J11,J27,0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K35"/>
@@ -4985,21 +4995,21 @@
       </c>
       <c r="D36" s="133"/>
       <c r="E36" s="133">
-        <f>IF(E12,E28,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="134"/>
+        <f t="shared" ref="D36:J36" si="9">IF(E12,E28,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="133"/>
       <c r="G36" s="133">
-        <f>IF(G12,G28,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H36" s="133"/>
       <c r="I36" s="133">
-        <f>IF(I12,I28,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J36" s="133">
-        <f>IF(J12,J28,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5016,404 +5026,370 @@
       </c>
       <c r="D37" s="133"/>
       <c r="E37" s="133">
-        <f t="shared" ref="E37" si="7">E36+E35+E34</f>
+        <f t="shared" ref="D37:J37" si="10">E36+E35+E34</f>
         <v>9.1168831168831179</v>
       </c>
-      <c r="F37" s="134"/>
+      <c r="F37" s="133"/>
       <c r="G37" s="133">
-        <f>G36+G35+G34</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H37" s="133"/>
       <c r="I37" s="133">
-        <f>I36+I35+I34</f>
+        <f t="shared" si="10"/>
         <v>15.600000000000001</v>
       </c>
       <c r="J37" s="133">
-        <f>J36+J35+J34</f>
+        <f t="shared" si="10"/>
         <v>7.5974025974025983</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="124" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B38" s="118"/>
       <c r="C38" s="133">
-        <f>C37*MIN(C7:C8)</f>
-        <v>527.67000000000007</v>
+        <f>C6-C34</f>
+        <v>-1.7000000000000011</v>
       </c>
       <c r="D38" s="133"/>
       <c r="E38" s="133">
-        <f>E37*MIN(E7:E8)</f>
-        <v>205.58571428571432</v>
-      </c>
-      <c r="F38" s="134"/>
+        <f t="shared" ref="D38:J38" si="11">E6-E34</f>
+        <v>7.1831168831168828</v>
+      </c>
+      <c r="F38" s="133"/>
       <c r="G38" s="133">
-        <f>G37*MIN(G7:G8)</f>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>10</v>
       </c>
       <c r="H38" s="133"/>
       <c r="I38" s="133">
-        <f>I37*MIN(I7:I8)</f>
-        <v>982.80000000000007</v>
+        <f t="shared" si="11"/>
+        <v>0.69999999999999929</v>
       </c>
       <c r="J38" s="133">
-        <f>J37*MIN(J7:J8)</f>
-        <v>562.2837662337663</v>
+        <f t="shared" si="11"/>
+        <v>2.4025974025974017</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="118" t="s">
-        <v>49</v>
-      </c>
+      <c r="A39" s="124" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="118"/>
       <c r="C39" s="133">
-        <f>(C6*MIN(C7:C8))-C38</f>
-        <v>-76.670000000000073</v>
+        <v>0.7</v>
       </c>
       <c r="D39" s="133"/>
       <c r="E39" s="133">
-        <f>(E6*MIN(E7:E8))-E38</f>
-        <v>161.97928571428574</v>
-      </c>
-      <c r="F39" s="134"/>
+        <v>0.7</v>
+      </c>
+      <c r="F39" s="133"/>
       <c r="G39" s="133">
-        <f>(G6*MIN(G7:G8))-G38</f>
-        <v>1500</v>
+        <v>0.7</v>
       </c>
       <c r="H39" s="133"/>
       <c r="I39" s="133">
-        <f>(I6*MIN(I7:I8))-I38</f>
-        <v>44.100000000000023</v>
+        <v>0.7</v>
       </c>
       <c r="J39" s="133">
-        <f>(J6*MIN(J7:J8))-J38</f>
-        <v>177.81623376623372</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="118" t="s">
-        <v>49</v>
-      </c>
+      <c r="A40" s="124" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="118"/>
       <c r="C40" s="133">
-        <f>0.7*MIN(C7:C8)</f>
-        <v>31.57</v>
+        <f>IF((C39-C38)&gt;=0,(C39-C38),0)</f>
+        <v>2.4000000000000012</v>
       </c>
       <c r="D40" s="133"/>
       <c r="E40" s="133">
-        <f>0.7*MIN(E7:E8)</f>
-        <v>15.785</v>
-      </c>
-      <c r="F40" s="134"/>
+        <f t="shared" ref="D40:J40" si="12">IF((E39-E38)&gt;=0,(E39-E38),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="133"/>
       <c r="G40" s="133">
-        <f>0.7*MIN(G7:G8)</f>
-        <v>105</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="H40" s="133"/>
       <c r="I40" s="133">
-        <f>0.7*MIN(I7:I8)</f>
-        <v>44.099999999999994</v>
+        <f t="shared" si="12"/>
+        <v>6.6613381477509392E-16</v>
       </c>
       <c r="J40" s="133">
-        <f>0.7*MIN(J7:J8)</f>
-        <v>51.807000000000002</v>
-      </c>
-      <c r="K40" s="110" t="s">
-        <v>34</v>
-      </c>
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="110"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="118" t="s">
-        <v>49</v>
-      </c>
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="118"/>
       <c r="C41" s="133">
-        <f>IF((C40-C39)&gt;=0,(C40-C39),0)</f>
-        <v>108.24000000000007</v>
+        <f>C34-C40</f>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D41" s="133"/>
       <c r="E41" s="133">
-        <f t="shared" ref="E41" si="8">IF((E40-E39)&gt;=0,(E40-E39),0)</f>
-        <v>0</v>
-      </c>
-      <c r="F41" s="134"/>
+        <f>E34-E40</f>
+        <v>9.1168831168831179</v>
+      </c>
+      <c r="F41" s="133"/>
       <c r="G41" s="133">
-        <f>IF((G40-G39)&gt;=0,(G40-G39),0)</f>
+        <f t="shared" ref="D41:J41" si="13">G34-G40</f>
         <v>0</v>
       </c>
       <c r="H41" s="133"/>
       <c r="I41" s="133">
-        <f>IF((I40-I39)&gt;=0,(I40-I39),0)</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>15.600000000000001</v>
       </c>
       <c r="J41" s="133">
-        <f t="shared" ref="J41" si="9">IF((J40-J39)&gt;=0,(J40-J39),0)</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>7.5974025974025983</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>43</v>
+      <c r="A42" t="s">
+        <v>86</v>
       </c>
       <c r="B42" s="118" t="s">
         <v>49</v>
       </c>
       <c r="C42" s="133">
-        <f>C38-C41</f>
-        <v>419.43</v>
+        <f>C10</f>
+        <v>0</v>
       </c>
       <c r="D42" s="133"/>
       <c r="E42" s="133">
-        <f t="shared" ref="E42" si="10">E38-E41</f>
-        <v>205.58571428571432</v>
-      </c>
-      <c r="F42" s="134"/>
+        <f t="shared" ref="D42:J42" si="14">E10</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="133"/>
       <c r="G42" s="133">
-        <f>G38-G41</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H42" s="133"/>
       <c r="I42" s="133">
-        <f>I38-I41</f>
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="133">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="134" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="135">
+        <f>C41+C42</f>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D43" s="135"/>
+      <c r="E43" s="135">
+        <f>E41+E42</f>
+        <v>9.1168831168831179</v>
+      </c>
+      <c r="F43" s="135"/>
+      <c r="G43" s="135">
+        <f t="shared" ref="D43:J43" si="15">G41+G42</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="135"/>
+      <c r="I43" s="135">
+        <f t="shared" si="15"/>
+        <v>15.600000000000001</v>
+      </c>
+      <c r="J43" s="135">
+        <f t="shared" si="15"/>
+        <v>9.5974025974025992</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="134" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="134" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="135">
+        <f>C43*MIN(C7:C8)</f>
+        <v>419.43000000000006</v>
+      </c>
+      <c r="D44" s="135"/>
+      <c r="E44" s="135">
+        <f>E43*MIN(E7:E8)</f>
+        <v>280.34415584415586</v>
+      </c>
+      <c r="F44" s="135"/>
+      <c r="G44" s="135">
+        <f t="shared" ref="D44:J44" si="16">G43*MIN(G7:G8)</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="135"/>
+      <c r="I44" s="135">
+        <f t="shared" si="16"/>
         <v>982.80000000000007</v>
       </c>
-      <c r="J42" s="133">
-        <f t="shared" ref="J42" si="11">J38-J41</f>
-        <v>562.2837662337663</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" s="118" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="133">
-        <f>C10*(MIN(C7:C8))</f>
-        <v>0</v>
-      </c>
-      <c r="D43" s="133"/>
-      <c r="E43" s="133">
-        <f>E10*(MIN(E7:E8))</f>
-        <v>0</v>
-      </c>
-      <c r="F43" s="134"/>
-      <c r="G43" s="133">
-        <f>G10*(MIN(G7:G8))</f>
-        <v>0</v>
-      </c>
-      <c r="H43" s="133"/>
-      <c r="I43" s="133">
-        <f>I10*(MIN(I7:I8))</f>
-        <v>0</v>
-      </c>
-      <c r="J43" s="133">
-        <f>J10*(MIN(J7:J8))</f>
-        <v>148.02000000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="135" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="135" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="136">
-        <f>C42+C43</f>
-        <v>419.43</v>
-      </c>
-      <c r="D44" s="136"/>
-      <c r="E44" s="136">
-        <f t="shared" ref="E44" si="12">E42+E43</f>
-        <v>205.58571428571432</v>
-      </c>
-      <c r="F44" s="137"/>
-      <c r="G44" s="136">
-        <f>G42+G43</f>
-        <v>0</v>
-      </c>
-      <c r="H44" s="136"/>
-      <c r="I44" s="136">
-        <f>I42+I43</f>
-        <v>982.80000000000007</v>
-      </c>
-      <c r="J44" s="136">
-        <f t="shared" ref="J44" si="13">J42+J43</f>
-        <v>710.30376623376628</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="135" t="s">
+      <c r="J44" s="135">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="135" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="136">
-        <f>C44/MIN(C7:C8)</f>
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="D45" s="136"/>
-      <c r="E45" s="136">
-        <f>E44/MIN(E7:E8)</f>
-        <v>9.1168831168831179</v>
-      </c>
-      <c r="F45" s="137"/>
-      <c r="G45" s="136">
-        <f>G44/MIN(G7:G8)</f>
-        <v>0</v>
-      </c>
-      <c r="H45" s="136"/>
-      <c r="I45" s="136">
-        <f>I44/MIN(I7:I8)</f>
-        <v>15.600000000000001</v>
-      </c>
-      <c r="J45" s="136">
-        <f>J44/MIN(J7:J8)</f>
-        <v>9.5974025974025974</v>
+      <c r="C46">
+        <f>C6*(MIN(C7:C8))</f>
+        <v>451</v>
+      </c>
+      <c r="E46">
+        <f t="shared" ref="D46:J46" si="17">E6*(MIN(E7:E8))</f>
+        <v>501.22500000000002</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="17"/>
+        <v>1500</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="17"/>
+        <v>1026.9000000000001</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47">
-        <f>C6*(MIN(C7:C8))</f>
-        <v>451</v>
-      </c>
-      <c r="E47">
-        <f>E6*(MIN(E7:E8))</f>
-        <v>367.56500000000005</v>
-      </c>
-      <c r="G47" s="140">
-        <f>G6*(MIN(G7:G8))</f>
-        <v>1500</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C47" s="59">
+        <f>SUM(C42,C37)</f>
+        <v>11.700000000000001</v>
+      </c>
+      <c r="D47" s="59"/>
+      <c r="E47" s="59">
+        <f t="shared" ref="D47:J47" si="18">SUM(E42,E37)</f>
+        <v>9.1168831168831179</v>
+      </c>
+      <c r="F47" s="59"/>
+      <c r="G47" s="59">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="H47" s="59"/>
       <c r="I47" s="59">
-        <f>I6*(MIN(I7:I8))</f>
-        <v>1026.9000000000001</v>
-      </c>
-      <c r="J47">
-        <f>J6*(MIN(J7:J8))</f>
-        <v>740.1</v>
+        <f t="shared" si="18"/>
+        <v>15.600000000000001</v>
+      </c>
+      <c r="J47" s="59">
+        <f t="shared" si="18"/>
+        <v>9.5974025974025992</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C48" s="59">
-        <f>SUM(C43,C38)</f>
-        <v>527.67000000000007</v>
-      </c>
-      <c r="D48" s="59"/>
+        <f>IF(C38&lt;0,C37+C38,C37)</f>
+        <v>10</v>
+      </c>
+      <c r="D48" s="59">
+        <f t="shared" ref="D48:J48" si="19">IF(D38&lt;0,D37+D38,D37)</f>
+        <v>0</v>
+      </c>
       <c r="E48" s="59">
-        <f t="shared" ref="E48" si="14">SUM(E43,E38)</f>
-        <v>205.58571428571432</v>
+        <f t="shared" si="19"/>
+        <v>9.1168831168831179</v>
+      </c>
+      <c r="F48" s="59">
+        <f t="shared" si="19"/>
+        <v>0</v>
       </c>
       <c r="G48" s="59">
-        <f>SUM(G43,G38)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="H48" s="59"/>
       <c r="I48" s="59">
-        <f>SUM(I43,I38)</f>
-        <v>982.80000000000007</v>
+        <f t="shared" si="19"/>
+        <v>15.600000000000001</v>
       </c>
       <c r="J48" s="59">
-        <f t="shared" ref="J48" si="15">SUM(J43,J38)</f>
-        <v>710.30376623376628</v>
+        <f t="shared" si="19"/>
+        <v>7.5974025974025983</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C49" s="59">
-        <f>IF(C39&lt;0,C38+C39,C38)+C43</f>
-        <v>451</v>
+        <f>C40</f>
+        <v>2.4000000000000012</v>
       </c>
       <c r="D49" s="59"/>
       <c r="E49" s="59">
-        <f t="shared" ref="E49" si="16">IF(E39&lt;0,E38+E39,E38)+E43</f>
-        <v>205.58571428571432</v>
-      </c>
+        <f t="shared" ref="D49:J49" si="20">E40</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="59"/>
       <c r="G49" s="59">
-        <f>IF(G39&lt;0,G38+G39,G38)+G43</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H49" s="59"/>
       <c r="I49" s="59">
-        <f>IF(I39&lt;0,I38+I39,I38)+I43</f>
-        <v>982.80000000000007</v>
+        <f t="shared" si="20"/>
+        <v>6.6613381477509392E-16</v>
       </c>
       <c r="J49" s="59">
-        <f t="shared" ref="J49" si="17">IF(J39&lt;0,J38+J39,J38)+J43</f>
-        <v>710.30376623376628</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C50" s="59">
-        <f>IF(C40&gt;C41,C41,C40)</f>
-        <v>31.57</v>
+        <f>C44</f>
+        <v>419.43000000000006</v>
       </c>
       <c r="D50" s="59"/>
       <c r="E50" s="59">
-        <f t="shared" ref="E50" si="18">IF(E40&gt;E41,E41,E40)</f>
-        <v>0</v>
-      </c>
+        <f t="shared" ref="D50:J50" si="21">E44</f>
+        <v>280.34415584415586</v>
+      </c>
+      <c r="F50" s="59"/>
       <c r="G50" s="59">
-        <f>IF(G40&gt;G41,G41,G40)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="H50" s="59"/>
       <c r="I50" s="59">
-        <f>IF(I40&gt;I41,I41,I40)</f>
-        <v>0</v>
+        <f t="shared" si="21"/>
+        <v>982.80000000000007</v>
       </c>
       <c r="J50" s="59">
-        <f t="shared" ref="J50" si="19">IF(J40&gt;J41,J41,J40)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="59">
-        <f>C49-C50</f>
-        <v>419.43</v>
-      </c>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59">
-        <f t="shared" ref="E51" si="20">E49-E50</f>
-        <v>205.58571428571432</v>
-      </c>
-      <c r="G51" s="59">
-        <f>G49-G50</f>
-        <v>0</v>
-      </c>
-      <c r="H51" s="59"/>
-      <c r="I51" s="59">
-        <f>I49-I50</f>
-        <v>982.80000000000007</v>
-      </c>
-      <c r="J51" s="59">
-        <f t="shared" ref="J51" si="21">J49-J50</f>
-        <v>710.30376623376628</v>
+        <f t="shared" si="21"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>